<commit_message>
big changes to data read in, parsing, storage, building duplicates still not working
</commit_message>
<xml_diff>
--- a/IEEE 39 Test Bus Data/IEEE_39_bus_data.xlsx
+++ b/IEEE 39 Test Bus Data/IEEE_39_bus_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlabecker/Library/Mobile Documents/com~apple~CloudDocs/Carla's Desktop/UC Berkeley/Spring 2024/CE 295 - Energy Systems and Control/CE295-OPF/IEEE 39 Test Bus Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA3F23E-3FD6-0B48-A3C4-6E82AD648AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997BE0D5-4FF0-0046-9475-7D59ED68B4B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-2760" windowWidth="51200" windowHeight="31500" activeTab="7" xr2:uid="{7BA741FC-404F-9246-8FCA-3A156079A65D}"/>
+    <workbookView xWindow="-51200" yWindow="-2760" windowWidth="51200" windowHeight="31500" activeTab="8" xr2:uid="{7BA741FC-404F-9246-8FCA-3A156079A65D}"/>
   </bookViews>
   <sheets>
     <sheet name="bus data" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="A matrix" sheetId="6" r:id="rId6"/>
     <sheet name="r matrix" sheetId="7" r:id="rId7"/>
     <sheet name="x matrix" sheetId="8" r:id="rId8"/>
+    <sheet name="rho" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>bus</t>
   </si>
@@ -139,6 +140,9 @@
   <si>
     <t>x_ij</t>
   </si>
+  <si>
+    <t>rho</t>
+  </si>
 </sst>
 </file>
 
@@ -184,307 +188,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="144">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="141">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1307,6 +1011,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1317,11 +1031,271 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4576,7 +4550,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L33" sqref="L33"/>
+      <selection pane="bottomRight" sqref="A1:AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11589,67 +11563,67 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:AN40 AO2:AV2">
-    <cfRule type="containsText" dxfId="143" priority="13" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="140" priority="13" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO3:AV47 AI41:AP47">
-    <cfRule type="containsText" dxfId="142" priority="12" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="139" priority="12" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AI3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W41:AD47">
-    <cfRule type="containsText" dxfId="141" priority="11" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="138" priority="11" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",W41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE41:AL47">
-    <cfRule type="containsText" dxfId="140" priority="10" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="137" priority="10" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AE41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O41:V47">
-    <cfRule type="containsText" dxfId="139" priority="9" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="136" priority="9" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",O41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41:N47">
-    <cfRule type="containsText" dxfId="138" priority="8" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="135" priority="8" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",J41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41:I47">
-    <cfRule type="containsText" dxfId="137" priority="7" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="134" priority="7" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI48:AV48">
-    <cfRule type="containsText" dxfId="136" priority="6" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="133" priority="6" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AI48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W48:AD48">
-    <cfRule type="containsText" dxfId="135" priority="5" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="132" priority="5" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",W48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE48:AL48">
-    <cfRule type="containsText" dxfId="134" priority="4" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="131" priority="4" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AE48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O48:V48">
-    <cfRule type="containsText" dxfId="133" priority="3" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="130" priority="3" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",O48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J48:N48">
-    <cfRule type="containsText" dxfId="132" priority="2" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="129" priority="2" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",J48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:I48">
-    <cfRule type="containsText" dxfId="131" priority="1" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="128" priority="1" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18725,70 +18699,70 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:AN40">
-    <cfRule type="beginsWith" dxfId="130" priority="46" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="127" priority="46" operator="beginsWith" text="??">
       <formula>LEFT(B2,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="126" priority="47" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI41:AN43 AI47:AK47 AJ44:AN44 AI45 AK45:AN45 AI46:AJ46 AL46:AN46 AM47:AN47">
-    <cfRule type="containsText" dxfId="128" priority="45" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="125" priority="45" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AI41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W41:AD44 W47:Y47 X45:AD45 W46 Y46:AD46 AA47:AD47">
-    <cfRule type="containsText" dxfId="127" priority="44" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="124" priority="44" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",W41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE47:AK47 AF41:AL41 AE42:AF42 AH42:AL42 AE43:AG43 AI43:AL43 AE44:AH44 AJ44:AL44 AE45:AI45 AK45:AL45 AE46:AJ46 AL46">
-    <cfRule type="containsText" dxfId="126" priority="43" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="123" priority="43" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AE41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O41:V42 O45:V47 O43:S43 U43:V43 O44:T44 V44">
-    <cfRule type="containsText" dxfId="125" priority="42" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="122" priority="42" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",O41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41:N41 J43:N47 J42 L42:N42">
-    <cfRule type="containsText" dxfId="124" priority="41" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="121" priority="41" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",J41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41:I47">
-    <cfRule type="containsText" dxfId="123" priority="40" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="120" priority="40" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI48:AL48 AN48">
-    <cfRule type="containsText" dxfId="122" priority="39" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="119" priority="39" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AI48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W48:AC48">
-    <cfRule type="containsText" dxfId="121" priority="38" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="118" priority="38" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",W48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE48:AL48">
-    <cfRule type="containsText" dxfId="120" priority="37" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="117" priority="37" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AE48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O48:V48">
-    <cfRule type="containsText" dxfId="119" priority="36" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="116" priority="36" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",O48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J48:N48">
-    <cfRule type="containsText" dxfId="118" priority="35" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="115" priority="35" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",J48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:I48">
-    <cfRule type="containsText" dxfId="117" priority="34" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="114" priority="34" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18808,122 +18782,122 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="beginsWith" dxfId="93" priority="29" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="110" priority="29" operator="beginsWith" text="??">
       <formula>LEFT(K42,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="109" priority="30" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T43">
-    <cfRule type="beginsWith" dxfId="91" priority="27" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="108" priority="27" operator="beginsWith" text="??">
       <formula>LEFT(T43,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U44">
-    <cfRule type="beginsWith" dxfId="89" priority="25" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="106" priority="25" operator="beginsWith" text="??">
       <formula>LEFT(U44,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="26" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W45">
-    <cfRule type="beginsWith" dxfId="87" priority="23" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="104" priority="23" operator="beginsWith" text="??">
       <formula>LEFT(W45,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="103" priority="24" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X46">
-    <cfRule type="beginsWith" dxfId="85" priority="21" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="102" priority="21" operator="beginsWith" text="??">
       <formula>LEFT(X46,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="22" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z47">
-    <cfRule type="beginsWith" dxfId="83" priority="19" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="100" priority="19" operator="beginsWith" text="??">
       <formula>LEFT(Z47,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="20" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD48">
-    <cfRule type="beginsWith" dxfId="81" priority="17" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="98" priority="17" operator="beginsWith" text="??">
       <formula>LEFT(AD48,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE41">
-    <cfRule type="beginsWith" dxfId="79" priority="15" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="96" priority="15" operator="beginsWith" text="??">
       <formula>LEFT(AE41,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="95" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG42">
-    <cfRule type="beginsWith" dxfId="77" priority="13" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="94" priority="13" operator="beginsWith" text="??">
       <formula>LEFT(AG42,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="93" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH43">
-    <cfRule type="beginsWith" dxfId="75" priority="11" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="92" priority="11" operator="beginsWith" text="??">
       <formula>LEFT(AH43,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="91" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI44">
-    <cfRule type="beginsWith" dxfId="73" priority="9" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="90" priority="9" operator="beginsWith" text="??">
       <formula>LEFT(AI44,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ45">
-    <cfRule type="beginsWith" dxfId="71" priority="7" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="88" priority="7" operator="beginsWith" text="??">
       <formula>LEFT(AJ45,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="87" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK46">
-    <cfRule type="beginsWith" dxfId="69" priority="5" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="86" priority="5" operator="beginsWith" text="??">
       <formula>LEFT(AK46,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="85" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL47">
-    <cfRule type="beginsWith" dxfId="67" priority="3" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="84" priority="3" operator="beginsWith" text="??">
       <formula>LEFT(AL47,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM48">
-    <cfRule type="beginsWith" dxfId="65" priority="1" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="82" priority="1" operator="beginsWith" text="??">
       <formula>LEFT(AM48,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="81" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18935,7 +18909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D57F7F03-0125-154D-9125-9AD5B612047B}">
   <dimension ref="A1:AV67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="Y61" sqref="Y61"/>
     </sheetView>
@@ -26003,85 +25977,85 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:AN40">
-    <cfRule type="beginsWith" dxfId="110" priority="80" operator="beginsWith" text="??">
+    <cfRule type="beginsWith" dxfId="80" priority="80" operator="beginsWith" text="??">
       <formula>LEFT(B2,LEN("??"))="??"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="81" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="79" priority="81" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AV2">
-    <cfRule type="containsText" dxfId="108" priority="79" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="78" priority="79" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AO2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO4:AV10 AO33:AV33 AP31:AV31 AO32 AQ32:AV32 AO40:AV47 AO34:AP34 AR34:AV34 AO35:AQ35 AS35:AV35 AO36:AR36 AT36:AV36 AO37:AS37 AU37:AV37 AO38:AT38 AV38 AO39:AU39 AO30:AU30 AO27:AV29 AO26:AT26 AV26 AO25:AV25 AO24:AS24 AU24:AV24 AO23:AR23 AT23:AV23 AO22:AV22 AO21:AQ21 AS21:AV21 AO20:AP20 AR20:AV20 AO12:AV19 AO11 AQ11:AV11 AP3:AV3">
-    <cfRule type="containsText" dxfId="107" priority="78" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="77" priority="78" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AO3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO48:AV48">
-    <cfRule type="containsText" dxfId="106" priority="77" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AO48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI41:AN43 AI47:AK47 AJ44:AN44 AI45 AK45:AN45 AI46:AJ46 AL46:AN46 AM47:AN47">
-    <cfRule type="containsText" dxfId="105" priority="76" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="75" priority="76" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AI41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W41:AD44 W46 X45:AD45 W47:Y47 AA47:AD47 Y46:AD46">
-    <cfRule type="containsText" dxfId="104" priority="75" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="74" priority="75" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",W41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE47:AK47 AF41:AL41 AE42:AF42 AH42:AL42 AE43:AG43 AI43:AL43 AE44:AH44 AJ44:AL44 AE45:AI45 AK45:AL45 AE46:AJ46 AL46">
-    <cfRule type="containsText" dxfId="103" priority="74" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AE41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O41:V42 O45:V47 O43:S43 U43:V43 O44:T44 V44">
-    <cfRule type="containsText" dxfId="102" priority="73" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="72" priority="73" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",O41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41:N41 J43:N47 J42 L42:N42">
-    <cfRule type="containsText" dxfId="101" priority="72" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="71" priority="72" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",J41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42:I47 B41 D41:I41">
-    <cfRule type="containsText" dxfId="100" priority="71" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI48:AL48 AN48">
-    <cfRule type="containsText" dxfId="99" priority="70" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="69" priority="70" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AI48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W48:AC48">
-    <cfRule type="containsText" dxfId="98" priority="69" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="68" priority="69" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",W48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE48:AL48">
-    <cfRule type="containsText" dxfId="97" priority="68" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AE48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O48:V48">
-    <cfRule type="containsText" dxfId="96" priority="67" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="66" priority="67" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",O48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J48:N48">
-    <cfRule type="containsText" dxfId="95" priority="66" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="65" priority="66" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",J48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:I48">
-    <cfRule type="containsText" dxfId="94" priority="65" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26343,4 +26317,752 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA937FD5-99DA-114A-9F6D-56A654897801}">
+  <dimension ref="A1:AV5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="49" width="3.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
+      <c r="AA1">
+        <v>26</v>
+      </c>
+      <c r="AB1">
+        <v>27</v>
+      </c>
+      <c r="AC1">
+        <v>28</v>
+      </c>
+      <c r="AD1">
+        <v>29</v>
+      </c>
+      <c r="AE1">
+        <v>30</v>
+      </c>
+      <c r="AF1">
+        <v>31</v>
+      </c>
+      <c r="AG1">
+        <v>32</v>
+      </c>
+      <c r="AH1">
+        <v>33</v>
+      </c>
+      <c r="AI1">
+        <v>34</v>
+      </c>
+      <c r="AJ1">
+        <v>35</v>
+      </c>
+      <c r="AK1">
+        <v>36</v>
+      </c>
+      <c r="AL1">
+        <v>37</v>
+      </c>
+      <c r="AM1">
+        <v>38</v>
+      </c>
+      <c r="AN1">
+        <v>39</v>
+      </c>
+      <c r="AO1">
+        <v>40</v>
+      </c>
+      <c r="AP1">
+        <v>41</v>
+      </c>
+      <c r="AQ1">
+        <v>42</v>
+      </c>
+      <c r="AR1">
+        <v>43</v>
+      </c>
+      <c r="AS1">
+        <v>44</v>
+      </c>
+      <c r="AT1">
+        <v>45</v>
+      </c>
+      <c r="AU1">
+        <v>46</v>
+      </c>
+      <c r="AV1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>8</v>
+      </c>
+      <c r="K2">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>6</v>
+      </c>
+      <c r="M2">
+        <v>11</v>
+      </c>
+      <c r="N2">
+        <v>10</v>
+      </c>
+      <c r="O2">
+        <v>4</v>
+      </c>
+      <c r="P2">
+        <v>14</v>
+      </c>
+      <c r="Q2">
+        <v>17</v>
+      </c>
+      <c r="R2">
+        <v>16</v>
+      </c>
+      <c r="S2">
+        <v>3</v>
+      </c>
+      <c r="T2">
+        <v>16</v>
+      </c>
+      <c r="U2">
+        <v>19</v>
+      </c>
+      <c r="V2">
+        <v>16</v>
+      </c>
+      <c r="W2">
+        <v>21</v>
+      </c>
+      <c r="X2">
+        <v>22</v>
+      </c>
+      <c r="Y2">
+        <v>16</v>
+      </c>
+      <c r="Z2">
+        <v>2</v>
+      </c>
+      <c r="AA2">
+        <v>25</v>
+      </c>
+      <c r="AB2">
+        <v>17</v>
+      </c>
+      <c r="AC2">
+        <v>26</v>
+      </c>
+      <c r="AD2">
+        <v>26</v>
+      </c>
+      <c r="AE2">
+        <v>2</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>10</v>
+      </c>
+      <c r="AH2">
+        <v>19</v>
+      </c>
+      <c r="AI2">
+        <v>20</v>
+      </c>
+      <c r="AJ2">
+        <v>22</v>
+      </c>
+      <c r="AK2">
+        <v>23</v>
+      </c>
+      <c r="AL2">
+        <v>25</v>
+      </c>
+      <c r="AM2">
+        <v>29</v>
+      </c>
+      <c r="AN2">
+        <v>1</v>
+      </c>
+      <c r="AO2">
+        <v>2</v>
+      </c>
+      <c r="AP2">
+        <v>10</v>
+      </c>
+      <c r="AQ2">
+        <v>19</v>
+      </c>
+      <c r="AR2">
+        <v>20</v>
+      </c>
+      <c r="AS2">
+        <v>22</v>
+      </c>
+      <c r="AT2">
+        <v>23</v>
+      </c>
+      <c r="AU2">
+        <v>25</v>
+      </c>
+      <c r="AV2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>9</v>
+      </c>
+      <c r="J3">
+        <v>39</v>
+      </c>
+      <c r="K3">
+        <v>13</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+      <c r="M3">
+        <v>13</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3">
+        <v>13</v>
+      </c>
+      <c r="P3">
+        <v>16</v>
+      </c>
+      <c r="Q3">
+        <v>19</v>
+      </c>
+      <c r="R3">
+        <v>18</v>
+      </c>
+      <c r="S3">
+        <v>17</v>
+      </c>
+      <c r="T3">
+        <v>20</v>
+      </c>
+      <c r="U3">
+        <v>34</v>
+      </c>
+      <c r="V3">
+        <v>22</v>
+      </c>
+      <c r="W3">
+        <v>23</v>
+      </c>
+      <c r="X3">
+        <v>24</v>
+      </c>
+      <c r="Y3">
+        <v>23</v>
+      </c>
+      <c r="Z3">
+        <v>26</v>
+      </c>
+      <c r="AA3">
+        <v>27</v>
+      </c>
+      <c r="AB3">
+        <v>26</v>
+      </c>
+      <c r="AC3">
+        <v>29</v>
+      </c>
+      <c r="AD3">
+        <v>28</v>
+      </c>
+      <c r="AE3">
+        <v>40</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>41</v>
+      </c>
+      <c r="AH3">
+        <v>42</v>
+      </c>
+      <c r="AI3">
+        <v>43</v>
+      </c>
+      <c r="AJ3">
+        <v>44</v>
+      </c>
+      <c r="AK3">
+        <v>45</v>
+      </c>
+      <c r="AL3">
+        <v>46</v>
+      </c>
+      <c r="AM3">
+        <v>47</v>
+      </c>
+      <c r="AN3">
+        <v>9</v>
+      </c>
+      <c r="AO3">
+        <v>30</v>
+      </c>
+      <c r="AP3">
+        <v>32</v>
+      </c>
+      <c r="AQ3">
+        <v>33</v>
+      </c>
+      <c r="AR3">
+        <v>34</v>
+      </c>
+      <c r="AS3">
+        <v>35</v>
+      </c>
+      <c r="AT3">
+        <v>36</v>
+      </c>
+      <c r="AU3">
+        <v>37</v>
+      </c>
+      <c r="AV3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>32</v>
+      </c>
+      <c r="L4">
+        <v>12</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>14</v>
+      </c>
+      <c r="O4">
+        <v>15</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>21</v>
+      </c>
+      <c r="R4">
+        <v>27</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>33</v>
+      </c>
+      <c r="U4">
+        <v>43</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>35</v>
+      </c>
+      <c r="X4">
+        <v>36</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>37</v>
+      </c>
+      <c r="AA4">
+        <v>28</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>38</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>0</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>31</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>41</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>24</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>42</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>44</v>
+      </c>
+      <c r="X5">
+        <v>45</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>46</v>
+      </c>
+      <c r="AA5">
+        <v>29</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>47</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>